<commit_message>
App performance vastly improved. Ready to send out for comments.
</commit_message>
<xml_diff>
--- a/data/data_def.xlsx
+++ b/data/data_def.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://drexel0-my.sharepoint.com/personal/lf649_drexel_edu/Documents/Research/IDEA Fellowship/Shiny_apps/SSP/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisafrueh/Library/CloudStorage/OneDrive-DrexelUniversity/Research/IDEA Fellowship/Shiny_apps/SSP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{1C550A83-04ED-7D42-9C0E-BFDA10BAAA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D37F2C4F-1A43-8446-9133-2BCDD2CB0860}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F194E9-AB6D-F04B-825D-5F8767CB76CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="2720" windowWidth="28040" windowHeight="16940" xr2:uid="{BA2D44AB-46B9-3A41-8230-8192DCED7AB1}"/>
+    <workbookView xWindow="380" yWindow="1060" windowWidth="28040" windowHeight="16940" xr2:uid="{BA2D44AB-46B9-3A41-8230-8192DCED7AB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>Variable</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Privileged Group</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>&lt;$25k annual income</t>
+  </si>
+  <si>
+    <t>ICE Dimension</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,13 +493,13 @@
         <v>25</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -510,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>